<commit_message>
doc and csvs updated
</commit_message>
<xml_diff>
--- a/result_without_async.xlsx
+++ b/result_without_async.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projs\ml_products_from_url\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0430601-3927-4125-A7F9-18377D3835DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3D93B7-3C13-4706-B446-9CF077E985FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="37660" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="4660" yWindow="1110" windowWidth="28080" windowHeight="15910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2304,6 +2304,846 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.2"/>
+          <c:y val="3.2407407407407406E-2"/>
+          <c:w val="0.53888888888888886"/>
+          <c:h val="0.89814814814814814"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$5:$C$6</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>FALSE</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>TRUE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:scene3d>
+                <a:camera prst="orthographicFront"/>
+                <a:lightRig rig="brightRoom" dir="t"/>
+              </a:scene3d>
+              <a:sp3d prstMaterial="flat">
+                <a:bevelT w="50800" h="101600" prst="angle"/>
+                <a:contourClr>
+                  <a:srgbClr val="000000"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:scene3d>
+                <a:camera prst="orthographicFront"/>
+                <a:lightRig rig="brightRoom" dir="t"/>
+              </a:scene3d>
+              <a:sp3d prstMaterial="flat">
+                <a:bevelT w="50800" h="101600" prst="angle"/>
+                <a:contourClr>
+                  <a:srgbClr val="000000"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$5:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>55.035460992907801</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44.964539007092199</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D1B0-46AD-B4B8-8D22DCCB46B6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="inEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="258">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:scene3d>
+        <a:camera prst="orthographicFront"/>
+        <a:lightRig rig="brightRoom" dir="t"/>
+      </a:scene3d>
+      <a:sp3d prstMaterial="flat">
+        <a:bevelT w="50800" h="101600" prst="angle"/>
+        <a:contourClr>
+          <a:srgbClr val="000000"/>
+        </a:contourClr>
+      </a:sp3d>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" i="0" kern="1200" cap="all" spc="50" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3175</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>168275</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>307975</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2AF7CFB3-CE0E-5CA7-1157-D30BABC8D505}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2593,10 +3433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D706"/>
+  <dimension ref="A1:E706"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="D4" sqref="D4:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2605,7 +3445,7 @@
     <col min="2" max="2" width="15.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2613,7 +3453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -2621,7 +3461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -2629,15 +3469,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D4">
+        <f>D5+D6</f>
+        <v>705</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -2651,8 +3495,12 @@
         <f>COUNTIF(B:B, FALSE)</f>
         <v>388</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E5">
+        <f>D5/D4 * 100</f>
+        <v>55.035460992907801</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -2666,8 +3514,12 @@
         <f>COUNTIF(B:B, TRUE)</f>
         <v>317</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="E6">
+        <f>D6/D4 * 100</f>
+        <v>44.964539007092199</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -2675,7 +3527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -2683,7 +3535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -2691,7 +3543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
@@ -2699,7 +3551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
@@ -2707,7 +3559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -2715,7 +3567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
@@ -2723,7 +3575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
@@ -2731,7 +3583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>24</v>
       </c>
@@ -2739,7 +3591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>30</v>
       </c>
@@ -8984,5 +9836,6 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId705"/>
+  <drawing r:id="rId706"/>
 </worksheet>
 </file>
</xml_diff>